<commit_message>
Writing the result in excel using hashmap
</commit_message>
<xml_diff>
--- a/src/test/resources/Output/Flights.xlsx
+++ b/src/test/resources/Output/Flights.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>DEPARTURE</t>
   </si>
@@ -26,28 +26,79 @@
     <t>PRICE</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>19:00</t>
   </si>
   <si>
+    <t>2h 55m</t>
+  </si>
+  <si>
+    <t>21:55</t>
+  </si>
+  <si>
+    <t>4,996</t>
+  </si>
+  <si>
+    <t>08:15</t>
+  </si>
+  <si>
+    <t>11:10</t>
+  </si>
+  <si>
     <t>17:05</t>
   </si>
   <si>
-    <t>08:15</t>
+    <t>20:00</t>
   </si>
   <si>
     <t>12:00</t>
   </si>
   <si>
+    <t>14:55</t>
+  </si>
+  <si>
     <t>16:00</t>
   </si>
   <si>
+    <t>4h 50m</t>
+  </si>
+  <si>
+    <t>20:50</t>
+  </si>
+  <si>
+    <t>6,518</t>
+  </si>
+  <si>
     <t>06:45</t>
   </si>
   <si>
+    <t>6h 05m</t>
+  </si>
+  <si>
+    <t>12:50</t>
+  </si>
+  <si>
     <t>14:25</t>
+  </si>
+  <si>
+    <t>6h 25m</t>
+  </si>
+  <si>
+    <t>6h 35m</t>
+  </si>
+  <si>
+    <t>22:35</t>
+  </si>
+  <si>
+    <t>7h 55m</t>
+  </si>
+  <si>
+    <t>23:55</t>
+  </si>
+  <si>
+    <t>12:40</t>
+  </si>
+  <si>
+    <t>8h 10m</t>
   </si>
 </sst>
 </file>
@@ -92,60 +143,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="E1:F10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="E1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="E2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3">
-      <c r="E3" t="s">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4">
-      <c r="E4" t="s">
-        <v>8</v>
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5">
-      <c r="E5" t="s">
-        <v>9</v>
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6">
-      <c r="E6" t="s">
-        <v>10</v>
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7">
-      <c r="E7" t="s">
-        <v>11</v>
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8">
-      <c r="E8" t="s">
-        <v>9</v>
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9">
-      <c r="E9" t="s">
-        <v>11</v>
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10">
-      <c r="E10" t="s">
-        <v>10</v>
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>